<commit_message>
UPDATE: New data files to import Bouvier data. The main paper in collaboration with Bouvier lab. is out so the data can be pushed to the data repository.  https://doi.org/10.1101/2020.04.20.052027
</commit_message>
<xml_diff>
--- a/g_protein_data/200204_inoue.xlsx
+++ b/g_protein_data/200204_inoue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esguerra/gpcrdb/gpcrdb_data/g_protein_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esguerra/gpcrdb/protwis_vagrant_ubuntu/shared/data/protwis/gpcr/g_protein_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED18C0EA-F5CA-7D42-BA82-27A473FC3317}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFABA397-71C7-9247-8C3B-979BBF62F40B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogRA" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2085" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="182">
   <si>
     <t>Log RAi (Mean)</t>
     <phoneticPr fontId="3"/>
@@ -733,15 +733,14 @@
     <t>GNA13</t>
   </si>
   <si>
-    <t>Emax, %AP-TGFα release (Mean)</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>n =</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>Receptor</t>
+  </si>
+  <si>
+    <t>Emax (Mean)</t>
   </si>
 </sst>
 </file>
@@ -1655,7 +1654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X150"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="13"/>
   <cols>
@@ -1696,9 +1695,11 @@
       <c r="X1" s="4"/>
     </row>
     <row r="2" spans="1:24" ht="14" thickBot="1">
-      <c r="A2" s="6"/>
+      <c r="A2" s="6" t="s">
+        <v>180</v>
+      </c>
       <c r="B2" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>5</v>
@@ -12735,9 +12736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="13"/>
   <cols>
@@ -12779,10 +12778,10 @@
     </row>
     <row r="2" spans="1:24" ht="14" thickBot="1">
       <c r="A2" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>168</v>
@@ -23819,9 +23818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X150"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="13"/>
   <cols>
@@ -23834,7 +23831,7 @@
     <row r="1" spans="1:24" ht="14" thickBot="1">
       <c r="B1" s="13"/>
       <c r="C1" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -23862,10 +23859,10 @@
     </row>
     <row r="2" spans="1:24" ht="14" thickBot="1">
       <c r="A2" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>168</v>

</xml_diff>